<commit_message>
Aggiornamento per test 474
Aggiornamento per test 474
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#VITALSOFTWAREXX/VitalSoftware/Isolab9002/2.1/accreditamento-checklist_V8.2.7.xlsx
+++ b/GATEWAY/A1#111#VITALSOFTWAREXX/VitalSoftware/Isolab9002/2.1/accreditamento-checklist_V8.2.7.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaa\progEst\VitalSW_RicetteElettroniche_FSE2\20251125_AccreditamentoLabERadiologia\accreditamento8.2.7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaa\progEst\VitalSW_RicetteElettroniche_FSE2\20251125_AccreditamentoLabERadiologia\accreditamento8.2.7\20260126_FilesAccreditamento\A1#111#VITALSOFTWAREXX\VitalSoftware\Isolab9002\2.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AA37F0-7632-4643-8691-E572081B18DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D4F320-F049-4B95-BADD-26BBDA2EA217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="291">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1141,6 +1141,12 @@
   </si>
   <si>
     <t>L'errore segnalato sul monitor va in coda di retry. Dopo 5 tentativi il problema viene memorizzato in un file che sara' gestito dal supporto tecnico.</t>
+  </si>
+  <si>
+    <t>071d63539fe17b2f626b3de4f01dca91</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8a6f32ad89d2f9bd4fa1a8ce3162293262f08e3282e492b0715dc8cc96cc6483.ff52e087f1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3215,10 +3221,10 @@
   <dimension ref="A1:W606"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="P10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="W15" sqref="W15"/>
+      <selection pane="bottomRight" activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3228,7 +3234,9 @@
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="63.85546875" customWidth="1"/>
     <col min="5" max="5" width="104.85546875" customWidth="1"/>
-    <col min="6" max="9" width="33.140625" customWidth="1"/>
+    <col min="6" max="7" width="33.140625" customWidth="1"/>
+    <col min="8" max="8" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" customWidth="1"/>
     <col min="10" max="10" width="27.140625" customWidth="1"/>
     <col min="11" max="18" width="36.42578125" customWidth="1"/>
     <col min="19" max="19" width="27.140625" customWidth="1"/>
@@ -5895,10 +5903,10 @@
         <v>220</v>
       </c>
       <c r="H49" s="37" t="s">
-        <v>221</v>
+        <v>289</v>
       </c>
       <c r="I49" s="42" t="s">
-        <v>222</v>
+        <v>290</v>
       </c>
       <c r="J49" s="38" t="s">
         <v>52</v>
@@ -12170,21 +12178,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BE9A258ADBC3EC4CBEB1E2AB9909207A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0284f501378927579289f00316ec8a74">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="295b7897-c886-40bf-9750-5782b814c3e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b47213d65be806e283915cff374a7eef" ns2:_="">
     <xsd:import namespace="295b7897-c886-40bf-9750-5782b814c3e4"/>
@@ -12328,32 +12321,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7568E770-0BC4-46AF-B6C6-958AE21C8F7F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12371,6 +12354,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{cf8c7287-838c-46dd-b281-b1140229e67a}" enabled="1" method="Privileged" siteId="{75e027c9-20d5-47d5-b82f-77d7cd041e8f}" contentBits="0" removed="0"/>

</xml_diff>